<commit_message>
re today 2026 01 08
</commit_message>
<xml_diff>
--- a/13_0108_コマンドライン引数・ライブラリ/work2/sincurve.xlsx
+++ b/13_0108_コマンドライン引数・ライブラリ/work2/sincurve.xlsx
@@ -5,16 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoshitosuzuki/Library/Mobile Documents/com~apple~CloudDocs/university/byClass/2ndS/43プログラミング基礎演習/code/13_0108_コマンドライン引数・ライブラリ/work1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoshitosuzuki/Library/Mobile Documents/com~apple~CloudDocs/university/byClass/2ndS/43プログラミング基礎演習/code/13_0108_コマンドライン引数・ライブラリ/work2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E3AC6D3-7884-764D-93B8-19A02340A1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AE7CB73-379F-B849-88BE-B88A37073186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="1140" windowWidth="27900" windowHeight="16780" xr2:uid="{7008EC43-D4B1-674C-A8B2-CD98E6EE5302}"/>
   </bookViews>
   <sheets>
     <sheet name="sincurve" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">sincurve!$A$1:$A$100</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">sincurve!$B$1:$B$100</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">sincurve!$A$1:$A$100</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">sincurve!$B$1:$B$100</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -669,6 +675,1569 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>sincurve!$A$1:$A$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.32</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.44</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.56</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.62</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.68</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.86</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.16</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.2200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.2799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.34</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.46</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.52</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.58</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.82</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.94</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.12</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.18</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.24</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.36</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.48</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.54</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.72</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.78</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.84</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.96</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4.1399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.26</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4.32</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.38</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.4400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.5599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.62</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4.68</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.74</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4.8600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.92</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5.04</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5.16</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5.22</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>5.28</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>5.34</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.52</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5.58</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5.64</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.76</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5.82</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>5.88</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>5.94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>sincurve!$B$1:$B$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9964000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.119712</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17902999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.237703</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29552</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35227399999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.40776000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.461779</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.51413600000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.56464199999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.61311700000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.659385</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.70327899999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.74464300000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.783327</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.81919200000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85210799999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.88195800000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.90863300000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.93203899999999995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.95208999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.96871499999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.981854</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99145799999999995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99749500000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.999942</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99878999999999996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.99404300000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.98571900000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.97384800000000005</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.95847099999999996</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.93964499999999995</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.91743799999999998</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.89192899999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.863209</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.83138299999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.79656499999999997</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.75888100000000003</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.71846500000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.67546300000000004</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.63003100000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.58233100000000004</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.53253499999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.480823</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.42737999999999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.37239899999999998</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.31607800000000003</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.25861899999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.20022999999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.14112</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.1502000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.1590999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-3.8398000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-9.8249000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-0.157746</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-0.21667500000000001</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-0.27482499999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-0.33198499999999997</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-0.38795099999999999</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-0.44252000000000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-0.49549700000000002</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-0.54669100000000004</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-0.59591700000000003</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-0.64299899999999999</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-0.68776599999999999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-0.73005799999999998</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-0.76972300000000005</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-0.80661799999999995</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-0.84060900000000005</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-0.87157600000000002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-0.89940500000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-0.92399799999999999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-0.94526600000000005</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-0.96313099999999996</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-0.97753000000000001</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-0.98841100000000004</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-0.99573500000000004</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-0.99947600000000003</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-0.99961900000000004</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-0.99616499999999997</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-0.98912500000000003</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-0.97852600000000001</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-0.96440499999999996</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-0.94681400000000004</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-0.92581500000000005</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-0.90148399999999995</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-0.87390800000000002</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-0.84318800000000005</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-0.80943299999999996</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-0.77276400000000001</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-0.73331500000000005</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-0.69122700000000004</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-0.64665099999999998</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-0.59974700000000003</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-0.55068600000000001</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-0.49964199999999998</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-0.44679999999999997</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-0.39234999999999998</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-0.33648800000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-93AA-794A-B088-951060D03BE5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="761028032"/>
+        <c:axId val="761022656"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="761028032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>x</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="761022656"/>
+        <c:crossesAt val="-1"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="761022656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="-1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>sin(x)</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="761028032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FDF8548-511C-2108-4C29-46E553BBD644}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -1795,5 +3364,6 @@
   </sheetData>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>